<commit_message>
create API for defense
</commit_message>
<xml_diff>
--- a/server/files/Danh_sach_de_tai_cac_nhom.xlsx
+++ b/server/files/Danh_sach_de_tai_cac_nhom.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -59,6 +59,15 @@
     <t>demo</t>
   </si>
   <si>
+    <t>3333332123</t>
+  </si>
+  <si>
+    <t>Van</t>
+  </si>
+  <si>
+    <t>3333332121</t>
+  </si>
+  <si>
     <t>3333333221</t>
   </si>
   <si>
@@ -68,13 +77,37 @@
     <t>Le</t>
   </si>
   <si>
-    <t>3333332121</t>
-  </si>
-  <si>
-    <t>Van</t>
-  </si>
-  <si>
-    <t>3333332123</t>
+    <t>2512512112</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>Demo1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>0921525812</t>
+  </si>
+  <si>
+    <t>9316712115</t>
+  </si>
+  <si>
+    <t>0921525813</t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>2205612617</t>
+  </si>
+  <si>
+    <t>2342151123</t>
   </si>
 </sst>
 </file>
@@ -451,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -514,10 +547,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -537,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -563,13 +596,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -582,6 +615,162 @@
       </c>
       <c r="H5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update export file project
</commit_message>
<xml_diff>
--- a/server/files/Danh_sach_de_tai_cac_nhom.xlsx
+++ b/server/files/Danh_sach_de_tai_cac_nhom.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10507"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3238EDA9-8452-E449-82ED-F22C5021C6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Capstone 1" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Capstone 2" state="visible" r:id="rId5"/>
+    <sheet name="Capstone 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Capstone 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>No.</t>
   </si>
@@ -32,6 +36,9 @@
     <t>Group</t>
   </si>
   <si>
+    <t>Mentor</t>
+  </si>
+  <si>
     <t>Topic</t>
   </si>
   <si>
@@ -53,7 +60,13 @@
     <t>C1SE.21</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>null null,null null</t>
+  </si>
+  <si>
+    <t>Capstone 123</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>24211202634</t>
@@ -68,23 +81,53 @@
     <t>C1SE.23</t>
   </si>
   <si>
-    <t>Capstone 123</t>
-  </si>
-  <si>
-    <t>123</t>
+    <t>null null</t>
+  </si>
+  <si>
+    <t>24211208536</t>
+  </si>
+  <si>
+    <t>24211208533</t>
+  </si>
+  <si>
+    <t>Đậu Minh</t>
+  </si>
+  <si>
+    <t>Hoàng</t>
+  </si>
+  <si>
+    <t>C2SE.01</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times new roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +138,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,12 +146,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,127 +517,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50" style="1" customWidth="1"/>
+    <col min="9" max="9" width="75" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>